<commit_message>
Commit Cocktailcode and FLR -3
</commit_message>
<xml_diff>
--- a/Upkeep_v3/Upkeep_v3/Cocktail_World/Template/Cocktail Code.xlsx
+++ b/Upkeep_v3/Upkeep_v3/Cocktail_World/Template/Cocktail Code.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ee5802a9bf16156/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harsh Araple\Source\Repos\Compel-admin\Upkeep_v3_Projects\Upkeep_v3\Upkeep_v3\Cocktail_World\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57721455-FF18-419C-AC04-A0A8A6DFC526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731FB962-0051-4C18-AC5C-C6342875E294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{366A9457-32ED-491F-9EDB-FD7B836CDB2B}"/>
   </bookViews>
@@ -33,19 +33,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Cocktail</t>
   </si>
   <si>
-    <t>CocktailCode</t>
+    <t>License Name</t>
+  </si>
+  <si>
+    <t>Cocktail Code</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>ck</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +73,15 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,9 +105,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,27 +424,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4910D70-4B2C-45ED-B074-25546C53BAB7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>